<commit_message>
update museum of fine arts image
</commit_message>
<xml_diff>
--- a/public/data/schedule.xlsx
+++ b/public/data/schedule.xlsx
@@ -8,32 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidyoung/Desktop/CFT CP meeting 1/celeros-event-app/public/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4F5D4DE-843C-7442-89B1-E31AB5305D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B34A3951-41FA-F547-A390-01DF40839FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{EF323C95-967C-1441-B022-8AAA733F5383}"/>
+    <workbookView xWindow="1500" yWindow="1400" windowWidth="27640" windowHeight="16680" xr2:uid="{1D0311D8-58C0-214D-A468-A1CD0D3726ED}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
   <si>
     <t>Day</t>
   </si>
@@ -62,116 +49,122 @@
     <t>Tag</t>
   </si>
   <si>
+    <t>Registration and Networking</t>
+  </si>
+  <si>
+    <t>Hyatt meeting room</t>
+  </si>
+  <si>
+    <t>Fabiana</t>
+  </si>
+  <si>
     <t>https://images.unsplash.com/photo-1560250097-0b93528c311a?q=80&amp;w=100&amp;auto=format&amp;fit=crop</t>
   </si>
   <si>
+    <t>Welcome, safety moment and Introductions</t>
+  </si>
+  <si>
+    <t>Global Updates &amp; 2026 Outlook</t>
+  </si>
+  <si>
+    <t>Jose Larios</t>
+  </si>
+  <si>
     <t>https://images.unsplash.com/photo-1573496359142-b8d87734a5a2?q=80&amp;w=100&amp;auto=format&amp;fit=crop</t>
   </si>
   <si>
-    <t>https://images.unsplash.com/photo-1472099645785-5658abf4ff4e?q=80&amp;w=100&amp;auto=format&amp;fit=crop</t>
-  </si>
-  <si>
-    <t>https://images.unsplash.com/photo-1580489944761-15a19d654956?q=80&amp;w=100&amp;auto=format&amp;fit=crop</t>
-  </si>
-  <si>
-    <t>https://images.unsplash.com/photo-1519085360753-af0119f7cbe7?q=80&amp;w=100&amp;auto=format&amp;fit=crop</t>
-  </si>
-  <si>
-    <t>Welcome, safety moment and Introductions</t>
-  </si>
-  <si>
-    <t>Global Updates &amp; 2026 Outlook</t>
-  </si>
-  <si>
     <t>2025 - Year in Review</t>
-  </si>
-  <si>
-    <t>Break</t>
-  </si>
-  <si>
-    <t>Factory Healkth Check</t>
-  </si>
-  <si>
-    <t>SAP Improvements/ Delivery Commitment/ OTD</t>
-  </si>
-  <si>
-    <t>Success Story from CP/ RSM</t>
-  </si>
-  <si>
-    <t>Supply Chain Enhancements/ Stocking Program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lunch </t>
-  </si>
-  <si>
-    <t>Engineering Updates/ Product Upgrades</t>
-  </si>
-  <si>
-    <t>Trade Compliance</t>
-  </si>
-  <si>
-    <t>Com Ops Improvements</t>
-  </si>
-  <si>
-    <t>Aftermarket</t>
-  </si>
-  <si>
-    <t>Product Mangement</t>
-  </si>
-  <si>
-    <t>Project Management</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>Round up of the day</t>
-  </si>
-  <si>
-    <t>Fabiana</t>
-  </si>
-  <si>
-    <t>Tommy Kasim</t>
-  </si>
-  <si>
-    <t>Jose Larios</t>
   </si>
   <si>
     <t>Ken Lazzara
 Pedro Flores</t>
   </si>
   <si>
+    <t>https://images.unsplash.com/photo-1472099645785-5658abf4ff4e?q=80&amp;w=100&amp;auto=format&amp;fit=crop</t>
+  </si>
+  <si>
+    <t>Break</t>
+  </si>
+  <si>
+    <t>Hyatt meeting room lobby</t>
+  </si>
+  <si>
+    <t>Factory Healkth Check</t>
+  </si>
+  <si>
     <t>Federico Medina</t>
   </si>
   <si>
+    <t>https://images.unsplash.com/photo-1580489944761-15a19d654956?q=80&amp;w=100&amp;auto=format&amp;fit=crop</t>
+  </si>
+  <si>
+    <t>SAP Improvements/ Delivery Commitment/ OTD</t>
+  </si>
+  <si>
     <t>Jeff Lyon</t>
   </si>
   <si>
+    <t>Success Story from CP/ RSM</t>
+  </si>
+  <si>
     <t>CP to decide</t>
   </si>
   <si>
+    <t>https://images.unsplash.com/photo-1519085360753-af0119f7cbe7?q=80&amp;w=100&amp;auto=format&amp;fit=crop</t>
+  </si>
+  <si>
+    <t>Supply Chain Enhancements/ Stocking Program</t>
+  </si>
+  <si>
     <t>Yulong Su</t>
   </si>
   <si>
+    <t xml:space="preserve">Lunch </t>
+  </si>
+  <si>
+    <t>Hyatt Dining room</t>
+  </si>
+  <si>
+    <t>Engineering Updates/ Product Upgrades</t>
+  </si>
+  <si>
     <t>Raul Almazan</t>
   </si>
   <si>
+    <t>Trade Compliance</t>
+  </si>
+  <si>
     <t>Ann Brown</t>
   </si>
   <si>
+    <t>Com Ops Improvements</t>
+  </si>
+  <si>
     <t>Sergio Moscon</t>
   </si>
   <si>
+    <t>Aftermarket</t>
+  </si>
+  <si>
     <t>David Young</t>
   </si>
   <si>
+    <t>Product Mangement</t>
+  </si>
+  <si>
     <t>Pedro Flores</t>
   </si>
   <si>
+    <t>Project Management</t>
+  </si>
+  <si>
     <t>Jose Ortiz</t>
   </si>
   <si>
-    <t>Registration and Networking</t>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Round up of the day</t>
   </si>
   <si>
     <t>Overview of CVK Product</t>
@@ -186,12 +179,21 @@
     <t>Sizing Tool</t>
   </si>
   <si>
+    <t>Kevin Teygart</t>
+  </si>
+  <si>
     <t>Product/Applications - Feed Water, Recirculation Valve</t>
   </si>
   <si>
+    <t>Ken Lazzara</t>
+  </si>
+  <si>
     <t>DSCV</t>
   </si>
   <si>
+    <t>Mark Wheat</t>
+  </si>
+  <si>
     <t>Desuperheater Overview</t>
   </si>
   <si>
@@ -201,18 +203,30 @@
     <t>Bus to factory</t>
   </si>
   <si>
+    <t>Meet Hotel Lobby</t>
+  </si>
+  <si>
     <t>Factory Tour</t>
   </si>
   <si>
+    <t>Westplain Facility</t>
+  </si>
+  <si>
     <t>Bus back to hotel</t>
   </si>
   <si>
+    <t>Factory meeting point</t>
+  </si>
+  <si>
     <t>Lunch</t>
   </si>
   <si>
     <t>Open for meetings</t>
   </si>
   <si>
+    <t>Meeting Room</t>
+  </si>
+  <si>
     <t>Roundup / Thoughts / Catchball</t>
   </si>
   <si>
@@ -222,43 +236,19 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Kevin Teygart</t>
-  </si>
-  <si>
-    <t>Ken Lazzara</t>
-  </si>
-  <si>
-    <t>Mark Wheat</t>
-  </si>
-  <si>
-    <t>Meet Hotel Lobby</t>
-  </si>
-  <si>
-    <t>Factory meeting point</t>
-  </si>
-  <si>
-    <t>Meeting Room</t>
-  </si>
-  <si>
-    <t>Hyatt meeting room</t>
-  </si>
-  <si>
-    <t>Hyatt meeting room lobby</t>
-  </si>
-  <si>
-    <t>Hyatt Dining room</t>
-  </si>
-  <si>
-    <t>Westplain Facility</t>
+    <t>Tommy Kassim</t>
+  </si>
+  <si>
+    <t>Ken Lazzara / Pedro Flores</t>
+  </si>
+  <si>
+    <t>Fabiana Fionda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[m]"/>
-  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -736,13 +726,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1117,21 +1106,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A7AD26-CA0F-AF48-8458-254EB86FEC2A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{536245D3-7A2C-F14E-96B9-14A262A8F857}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" customWidth="1"/>
-    <col min="7" max="7" width="25.5" customWidth="1"/>
-    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1171,20 +1155,19 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="3">
-        <f>TIME(0,45,0)</f>
-        <v>3.125E-2</v>
-      </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
@@ -1195,21 +1178,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <f>B2+E2</f>
         <v>0.36458333333333331</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="3">
-        <f>TIME(0,15,0)</f>
-        <v>1.0416666666666666E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -1220,52 +1201,48 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:B21" si="0">B3+E3</f>
         <v>0.375</v>
       </c>
       <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="3">
-        <f t="shared" ref="E4:E43" si="1">TIME(0,30,0)</f>
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="0"/>
         <v>0.39583333333333331</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -1276,18 +1253,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.41666666666666663</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
       </c>
       <c r="H6" t="b">
         <v>1</v>
@@ -1298,24 +1273,22 @@
         <v>1</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.43749999999999994</v>
+        <v>0.4375</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="3">
-        <f>TIME(0,15,0)</f>
-        <v>1.0416666666666666E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -1326,21 +1299,19 @@
         <v>1</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.44791666666666663</v>
+        <v>0.44791666666666669</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -1351,24 +1322,22 @@
         <v>1</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.46874999999999994</v>
+        <v>0.46875</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="3">
-        <f>TIME(0,15,0)</f>
-        <v>1.0416666666666666E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -1379,21 +1348,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="0"/>
-        <v>0.47916666666666663</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -1404,18 +1371,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="0"/>
-        <v>0.49999999999999994</v>
+        <v>0.5</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="3">
-        <f>TIME(0,60,0)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <v>60</v>
       </c>
       <c r="H11" t="b">
         <v>1</v>
@@ -1426,21 +1391,19 @@
         <v>1</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="0"/>
         <v>0.54166666666666663</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -1451,21 +1414,19 @@
         <v>1</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="0"/>
         <v>0.5625</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="3">
-        <f>TIME(0,15,0)</f>
-        <v>1.0416666666666666E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -1476,21 +1437,19 @@
         <v>1</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="0"/>
         <v>0.57291666666666663</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -1501,21 +1460,19 @@
         <v>1</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="0"/>
         <v>0.59375</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -1526,18 +1483,16 @@
         <v>1</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="0"/>
         <v>0.61458333333333337</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>21</v>
+      </c>
+      <c r="E16">
+        <v>30</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
@@ -1548,18 +1503,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="0"/>
-        <v>0.63541666666666674</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>30</v>
       </c>
       <c r="F17" t="s">
         <v>43</v>
@@ -1573,21 +1526,19 @@
         <v>1</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="0"/>
-        <v>0.65625000000000011</v>
+        <v>0.65625</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="3">
-        <f>TIME(0,15,0)</f>
-        <v>1.0416666666666666E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
@@ -1598,21 +1549,19 @@
         <v>1</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
-        <v>0.66666666666666674</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="3">
-        <f>TIME(0,15,0)</f>
-        <v>1.0416666666666666E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -1623,21 +1572,19 @@
         <v>1</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="0"/>
         <v>0.67708333333333337</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>30</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -1648,21 +1595,19 @@
         <v>1</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="0"/>
-        <v>0.69791666666666674</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="3">
-        <f>TIME(0,45,0)</f>
-        <v>3.125E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>45</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
@@ -1676,17 +1621,16 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="3">
-        <f>TIME(0,45,0)</f>
-        <v>3.125E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>45</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="H22" t="b">
         <v>1</v>
@@ -1697,18 +1641,16 @@
         <v>2</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" ref="B23:B43" si="2">B22+E22</f>
         <v>0.36458333333333331</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>30</v>
       </c>
       <c r="F23" t="s">
         <v>43</v>
@@ -1722,18 +1664,16 @@
         <v>2</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" si="2"/>
-        <v>0.38541666666666663</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>30</v>
       </c>
       <c r="F24" t="s">
         <v>43</v>
@@ -1742,26 +1682,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" si="2"/>
-        <v>0.40624999999999994</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>48</v>
+        <v>0.40625</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="3">
-        <f>TIME(0,15,0)</f>
-        <v>1.0416666666666666E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
@@ -1772,18 +1710,16 @@
         <v>2</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" si="2"/>
-        <v>0.41666666666666663</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>21</v>
+      </c>
+      <c r="E26">
+        <v>30</v>
       </c>
       <c r="H26" t="b">
         <v>1</v>
@@ -1794,21 +1730,19 @@
         <v>2</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" si="2"/>
-        <v>0.43749999999999994</v>
+        <v>0.4375</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="3">
-        <f>TIME(0,120,0)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E27">
+        <v>120</v>
       </c>
       <c r="F27" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="H27" t="b">
         <v>0</v>
@@ -1819,18 +1753,16 @@
         <v>2</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" si="2"/>
-        <v>0.52083333333333326</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="3">
-        <f>TIME(0,60,0)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>33</v>
+      </c>
+      <c r="E28">
+        <v>60</v>
       </c>
       <c r="H28" t="b">
         <v>1</v>
@@ -1841,21 +1773,19 @@
         <v>2</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" si="2"/>
-        <v>0.56249999999999989</v>
+        <v>0.5625</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <v>30</v>
       </c>
       <c r="F29" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="H29" t="b">
         <v>0</v>
@@ -1866,21 +1796,19 @@
         <v>2</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" si="2"/>
-        <v>0.58333333333333326</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" s="3">
-        <f>TIME(0,60,0)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>60</v>
       </c>
       <c r="F30" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="H30" t="b">
         <v>0</v>
@@ -1891,18 +1819,16 @@
         <v>2</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" si="2"/>
-        <v>0.62499999999999989</v>
+        <v>0.625</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E31" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>21</v>
+      </c>
+      <c r="E31">
+        <v>30</v>
       </c>
       <c r="H31" t="b">
         <v>1</v>
@@ -1913,46 +1839,42 @@
         <v>2</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" si="2"/>
-        <v>0.64583333333333326</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="C32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32">
+        <v>60</v>
+      </c>
+      <c r="F32" t="s">
         <v>52</v>
       </c>
-      <c r="D32" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="3">
-        <f>TIME(0,60,0)</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F32" t="s">
-        <v>62</v>
-      </c>
       <c r="H32" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33" s="1">
-        <f t="shared" si="2"/>
-        <v>0.68749999999999989</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>48</v>
+        <v>0.6875</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
       </c>
       <c r="D33" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" s="3">
-        <f>TIME(0,15,0)</f>
-        <v>1.0416666666666666E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>15</v>
       </c>
       <c r="F33" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
@@ -1963,171 +1885,156 @@
         <v>2</v>
       </c>
       <c r="B34" s="1">
-        <f t="shared" si="2"/>
-        <v>0.69791666666666652</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="3">
-        <f>TIME(0,30,0)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>30</v>
       </c>
       <c r="F34" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="H34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
       <c r="B35" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35">
+        <v>30</v>
       </c>
       <c r="H35" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" si="2"/>
-        <v>0.35416666666666663</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>54</v>
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C36" t="s">
+        <v>59</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>60</v>
+      </c>
+      <c r="E36">
+        <v>30</v>
       </c>
       <c r="H36" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
       <c r="B37" s="1">
-        <f t="shared" si="2"/>
-        <v>0.37499999999999994</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>55</v>
+        <v>0.375</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>71</v>
-      </c>
-      <c r="E37" s="3">
-        <f>TIME(0,150,0)</f>
-        <v>0.10416666666666667</v>
+        <v>62</v>
+      </c>
+      <c r="E37">
+        <v>150</v>
       </c>
       <c r="H37" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
       <c r="B38" s="1">
-        <f t="shared" si="2"/>
-        <v>0.47916666666666663</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>56</v>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C38" t="s">
+        <v>63</v>
       </c>
       <c r="D38" t="s">
-        <v>66</v>
-      </c>
-      <c r="E38" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>64</v>
+      </c>
+      <c r="E38">
+        <v>30</v>
       </c>
       <c r="H38" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
       <c r="B39" s="1">
-        <f t="shared" si="2"/>
-        <v>0.49999999999999994</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>57</v>
+        <v>0.5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>65</v>
       </c>
       <c r="D39" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="3">
-        <f>TIME(0,60,0)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>21</v>
+      </c>
+      <c r="E39">
+        <v>60</v>
       </c>
       <c r="H39" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3</v>
       </c>
       <c r="B40" s="1">
-        <f t="shared" si="2"/>
         <v>0.54166666666666663</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>58</v>
+      <c r="C40" t="s">
+        <v>66</v>
       </c>
       <c r="D40" t="s">
         <v>67</v>
       </c>
-      <c r="E40" s="3">
-        <f>TIME(0,105,0)</f>
-        <v>7.2916666666666671E-2</v>
+      <c r="E40">
+        <v>105</v>
       </c>
       <c r="H40" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3</v>
       </c>
       <c r="B41" s="1">
-        <f t="shared" si="2"/>
-        <v>0.61458333333333326</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>59</v>
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="C41" t="s">
+        <v>68</v>
       </c>
       <c r="D41" t="s">
         <v>67</v>
       </c>
-      <c r="E41" s="3">
-        <f>TIME(0,45,0)</f>
-        <v>3.125E-2</v>
+      <c r="E41">
+        <v>45</v>
       </c>
       <c r="F41" t="s">
         <v>43</v>
@@ -2136,48 +2043,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
       <c r="B42" s="1">
-        <f t="shared" si="2"/>
-        <v>0.64583333333333326</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>60</v>
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C42" t="s">
+        <v>69</v>
       </c>
       <c r="D42" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+      <c r="E42">
+        <v>30</v>
       </c>
       <c r="F42" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="H42" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
       <c r="B43" s="1">
-        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>61</v>
+      <c r="C43" t="s">
+        <v>70</v>
       </c>
       <c r="D43" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+      <c r="E43">
+        <v>30</v>
       </c>
       <c r="H43" t="b">
         <v>1</v>

</xml_diff>